<commit_message>
BJ-178: Remove S3 service, add accounting model
</commit_message>
<xml_diff>
--- a/src/main/resources/templates/provision_of_service_act.xlsx
+++ b/src/main/resources/templates/provision_of_service_act.xlsx
@@ -42,20 +42,7 @@
             <rFont val="Calibri"/>
             <family val="2"/>
           </rPr>
-          <t>jx:area(lastCell="E92")</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="A59" authorId="0">
-      <text>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color indexed="81"/>
-            <rFont val="Calibri"/>
-            <family val="2"/>
-          </rPr>
-          <t>jx:each(items="payments" var="payment" lastCell="E59")</t>
+          <t>jx:area(lastCell="E46")</t>
         </r>
       </text>
     </comment>
@@ -64,7 +51,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="46">
   <si>
     <t>Акт об оказании услуг</t>
   </si>
@@ -168,72 +155,55 @@
     <t>м.п.</t>
   </si>
   <si>
-    <t>Клиент:</t>
-  </si>
-  <si>
-    <t>Принято, 
-руб.</t>
-  </si>
-  <si>
-    <t>К зачислению, 
-руб.</t>
-  </si>
-  <si>
-    <t>ИТОГО:</t>
-  </si>
-  <si>
-    <t>???</t>
-  </si>
-  <si>
     <t xml:space="preserve">??? </t>
   </si>
   <si>
-    <t>к Договору № ??? от ???</t>
-  </si>
-  <si>
-    <t>${fromTime}</t>
-  </si>
-  <si>
-    <t>${toTime}</t>
-  </si>
-  <si>
-    <t>${payment.amount}</t>
-  </si>
-  <si>
-    <t>${payment.fee}</t>
-  </si>
-  <si>
-    <t>Комиссия, 
-руб.</t>
-  </si>
-  <si>
-    <t>№ платежа</t>
-  </si>
-  <si>
-    <t>${payment.invoice_id}.${payment.id}</t>
-  </si>
-  <si>
-    <t>${dateTimeParser.parse(payment.created_at)}</t>
-  </si>
-  <si>
-    <t>Реестр операций за период с</t>
-  </si>
-  <si>
-    <t>Дата/Время</t>
+    <t>${shopAccounting.fromTime}</t>
+  </si>
+  <si>
+    <t>${shopAccounting.toTime}</t>
+  </si>
+  <si>
+    <t>${shopAccounting.openingBalance}</t>
+  </si>
+  <si>
+    <t>${shopAccounting.closingBalance}</t>
+  </si>
+  <si>
+    <t>${shopAccounting.fundsAcquired}</t>
+  </si>
+  <si>
+    <t>${shopAccounting.feeCharged}</t>
+  </si>
+  <si>
+    <t>${shopAccounting.merchantId}</t>
+  </si>
+  <si>
+    <t>${shopAccounting.merchantName}</t>
+  </si>
+  <si>
+    <t>${shopAccounting.merchantRepresentativePosition} ${shopAccounting.merchantRepresentativeFullName}</t>
+  </si>
+  <si>
+    <t>${shopAccounting.merchantContractCreatedAt}</t>
+  </si>
+  <si>
+    <t>к Договору № ${shopAccounting.merchantContractId} от</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <numFmts count="5">
+  <numFmts count="6">
     <numFmt numFmtId="164" formatCode="#,##0.00&quot; &quot;;&quot;-&quot;#,##0.00&quot; &quot;"/>
     <numFmt numFmtId="165" formatCode="0000"/>
     <numFmt numFmtId="166" formatCode="#0\,00"/>
     <numFmt numFmtId="167" formatCode="dd/mm/yy\ h:mm;@"/>
     <numFmt numFmtId="168" formatCode="[$-FC19]dd\ mmmm\ yyyy\ \г\.;@"/>
+    <numFmt numFmtId="169" formatCode="dd\.mm\.yyyy"/>
   </numFmts>
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color indexed="8"/>
@@ -250,12 +220,6 @@
       <sz val="11"/>
       <color indexed="8"/>
       <name val="Calibri"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color indexed="81"/>
-      <name val="Calibri"/>
-      <family val="2"/>
     </font>
     <font>
       <b/>
@@ -296,7 +260,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="8">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -329,59 +293,11 @@
       <bottom/>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color indexed="8"/>
-      </left>
-      <right style="thin">
-        <color indexed="8"/>
-      </right>
-      <top style="thin">
-        <color indexed="8"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="8"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="8"/>
-      </left>
-      <right/>
-      <top style="thin">
-        <color indexed="8"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="8"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color indexed="8"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="8"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="thin">
-        <color auto="1"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="41">
+  <cellXfs count="43">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -409,34 +325,10 @@
     <xf numFmtId="49" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="165" fontId="0" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="2" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="49" fontId="2" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top"/>
     </xf>
-    <xf numFmtId="166" fontId="0" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="166" fontId="0" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="top"/>
-    </xf>
     <xf numFmtId="14" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
@@ -448,9 +340,6 @@
     </xf>
     <xf numFmtId="49" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="167" fontId="0" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top" wrapText="1"/>
@@ -465,17 +354,52 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
+    <xf numFmtId="168" fontId="5" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="168" fontId="5" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="168" fontId="6" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="167" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top"/>
+    </xf>
     <xf numFmtId="166" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top"/>
+    </xf>
+    <xf numFmtId="166" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="4" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="169" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="49" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
@@ -484,14 +408,8 @@
     <xf numFmtId="49" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="168" fontId="6" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="168" fontId="6" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="168" fontId="7" fillId="2" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1682,8 +1600,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G92"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" view="pageBreakPreview" topLeftCell="A33" zoomScale="60" workbookViewId="0">
-      <selection activeCell="E48" sqref="E48"/>
+    <sheetView showGridLines="0" tabSelected="1" view="pageBreakPreview" zoomScale="60" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1695,24 +1613,26 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="35" t="s">
+      <c r="A1" s="39" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="35"/>
-      <c r="C1" s="35"/>
-      <c r="D1" s="35"/>
-      <c r="E1" s="35"/>
+      <c r="B1" s="39"/>
+      <c r="C1" s="39"/>
+      <c r="D1" s="39"/>
+      <c r="E1" s="39"/>
       <c r="F1"/>
       <c r="G1"/>
     </row>
     <row r="2" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="34" t="s">
-        <v>40</v>
-      </c>
-      <c r="B2" s="34"/>
-      <c r="C2" s="34"/>
-      <c r="D2" s="34"/>
-      <c r="E2" s="34"/>
+      <c r="A2" s="42" t="s">
+        <v>45</v>
+      </c>
+      <c r="B2" s="42"/>
+      <c r="C2" s="42"/>
+      <c r="D2" s="37" t="s">
+        <v>44</v>
+      </c>
+      <c r="E2" s="36"/>
       <c r="F2"/>
       <c r="G2"/>
     </row>
@@ -1726,13 +1646,13 @@
       <c r="G3"/>
     </row>
     <row r="4" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="37" t="s">
+      <c r="A4" s="41" t="s">
         <v>1</v>
       </c>
-      <c r="B4" s="37"/>
-      <c r="C4" s="37"/>
-      <c r="D4" s="37"/>
-      <c r="E4" s="37"/>
+      <c r="B4" s="41"/>
+      <c r="C4" s="41"/>
+      <c r="D4" s="41"/>
+      <c r="E4" s="41"/>
       <c r="F4"/>
       <c r="G4"/>
     </row>
@@ -1741,7 +1661,9 @@
       <c r="B5" s="2"/>
       <c r="C5" s="2"/>
       <c r="D5" s="2"/>
-      <c r="E5" s="2"/>
+      <c r="E5" s="8" t="s">
+        <v>3</v>
+      </c>
       <c r="F5"/>
       <c r="G5"/>
     </row>
@@ -1751,24 +1673,19 @@
       </c>
       <c r="B6" s="2"/>
       <c r="C6" s="2"/>
-      <c r="D6" s="10" t="s">
-        <v>3</v>
-      </c>
-      <c r="E6" s="8" t="s">
-        <v>38</v>
+      <c r="D6" s="10"/>
+      <c r="E6" s="35" t="s">
+        <v>42</v>
       </c>
       <c r="F6"/>
       <c r="G6"/>
     </row>
-    <row r="7" spans="1:7" s="24" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="24" t="s">
+    <row r="7" spans="1:7" s="16" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A7" s="16" t="s">
         <v>4</v>
       </c>
-      <c r="D7" s="24" t="s">
+      <c r="E7" s="16" t="s">
         <v>5</v>
-      </c>
-      <c r="E7" s="24" t="s">
-        <v>38</v>
       </c>
     </row>
     <row r="8" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
@@ -1776,25 +1693,27 @@
       <c r="B8" s="2"/>
       <c r="C8" s="2"/>
       <c r="D8" s="10"/>
-      <c r="E8" s="24"/>
+      <c r="E8" s="16" t="s">
+        <v>41</v>
+      </c>
       <c r="F8"/>
       <c r="G8"/>
     </row>
     <row r="9" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="2"/>
       <c r="B9" s="2"/>
-      <c r="C9" s="26"/>
-      <c r="D9" s="26"/>
-      <c r="E9" s="26"/>
+      <c r="C9" s="17"/>
+      <c r="D9" s="17"/>
+      <c r="E9" s="17"/>
       <c r="F9"/>
       <c r="G9"/>
     </row>
     <row r="10" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="2"/>
       <c r="B10" s="2"/>
-      <c r="C10" s="26"/>
-      <c r="D10" s="26"/>
-      <c r="E10" s="26"/>
+      <c r="C10" s="17"/>
+      <c r="D10" s="34"/>
+      <c r="E10" s="17"/>
       <c r="F10"/>
       <c r="G10"/>
     </row>
@@ -1808,7 +1727,7 @@
       <c r="G11"/>
     </row>
     <row r="12" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="28" t="s">
+      <c r="A12" s="19" t="s">
         <v>6</v>
       </c>
       <c r="B12" s="2"/>
@@ -1819,7 +1738,7 @@
       <c r="G12"/>
     </row>
     <row r="13" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A13" s="28" t="s">
+      <c r="A13" s="19" t="s">
         <v>7</v>
       </c>
       <c r="B13" s="2"/>
@@ -1842,14 +1761,14 @@
       <c r="A15" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="B15" s="39" t="s">
-        <v>41</v>
-      </c>
-      <c r="C15" s="27" t="s">
+      <c r="B15" s="24" t="s">
+        <v>35</v>
+      </c>
+      <c r="C15" s="18" t="s">
         <v>9</v>
       </c>
-      <c r="D15" s="38" t="s">
-        <v>42</v>
+      <c r="D15" s="23" t="s">
+        <v>36</v>
       </c>
       <c r="E15" s="3" t="s">
         <v>10</v>
@@ -1867,7 +1786,7 @@
       <c r="G16"/>
     </row>
     <row r="17" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A17" s="28" t="s">
+      <c r="A17" s="19" t="s">
         <v>11</v>
       </c>
       <c r="B17" s="2"/>
@@ -1878,14 +1797,13 @@
       <c r="G17"/>
     </row>
     <row r="18" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A18" s="28" t="s">
+      <c r="A18" s="19" t="s">
         <v>12</v>
       </c>
       <c r="B18" s="2"/>
       <c r="C18" s="2"/>
-      <c r="D18" s="32">
-        <f>C60</f>
-        <v>0</v>
+      <c r="D18" s="33" t="s">
+        <v>39</v>
       </c>
       <c r="E18" s="5" t="s">
         <v>13</v>
@@ -1897,20 +1815,19 @@
       <c r="A19" s="2"/>
       <c r="B19" s="2"/>
       <c r="C19" s="2"/>
-      <c r="D19" s="6"/>
+      <c r="D19" s="32"/>
       <c r="E19" s="6"/>
       <c r="F19"/>
       <c r="G19"/>
     </row>
     <row r="20" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A20" s="28" t="s">
+      <c r="A20" s="19" t="s">
         <v>14</v>
       </c>
       <c r="B20" s="2"/>
       <c r="C20" s="2"/>
-      <c r="D20" s="32">
-        <f>D60</f>
-        <v>0</v>
+      <c r="D20" s="33" t="s">
+        <v>40</v>
       </c>
       <c r="E20" s="5" t="s">
         <v>13</v>
@@ -1919,7 +1836,7 @@
       <c r="G20"/>
     </row>
     <row r="21" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A21" s="28" t="s">
+      <c r="A21" s="19" t="s">
         <v>15</v>
       </c>
       <c r="B21" s="2"/>
@@ -1948,13 +1865,13 @@
       <c r="G23"/>
     </row>
     <row r="24" spans="1:7" ht="31" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A24" s="33" t="s">
+      <c r="A24" s="38" t="s">
         <v>16</v>
       </c>
-      <c r="B24" s="33"/>
-      <c r="C24" s="33"/>
-      <c r="D24" s="32">
-        <v>0</v>
+      <c r="B24" s="38"/>
+      <c r="C24" s="38"/>
+      <c r="D24" s="33" t="s">
+        <v>37</v>
       </c>
       <c r="E24" s="5" t="s">
         <v>13</v>
@@ -1963,14 +1880,13 @@
       <c r="G24"/>
     </row>
     <row r="25" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A25" s="36" t="s">
+      <c r="A25" s="40" t="s">
         <v>17</v>
       </c>
-      <c r="B25" s="36"/>
-      <c r="C25" s="36"/>
-      <c r="D25" s="32">
-        <f>C60</f>
-        <v>0</v>
+      <c r="B25" s="40"/>
+      <c r="C25" s="40"/>
+      <c r="D25" s="33" t="s">
+        <v>39</v>
       </c>
       <c r="E25" s="5" t="s">
         <v>18</v>
@@ -1979,14 +1895,13 @@
       <c r="G25"/>
     </row>
     <row r="26" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A26" s="36" t="s">
+      <c r="A26" s="40" t="s">
         <v>19</v>
       </c>
-      <c r="B26" s="36"/>
-      <c r="C26" s="36"/>
-      <c r="D26" s="32">
-        <f>D60</f>
-        <v>0</v>
+      <c r="B26" s="40"/>
+      <c r="C26" s="40"/>
+      <c r="D26" s="33" t="s">
+        <v>40</v>
       </c>
       <c r="E26" s="5" t="s">
         <v>18</v>
@@ -1995,12 +1910,12 @@
       <c r="G26"/>
     </row>
     <row r="27" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A27" s="36" t="s">
+      <c r="A27" s="40" t="s">
         <v>20</v>
       </c>
-      <c r="B27" s="36"/>
-      <c r="C27" s="36"/>
-      <c r="D27" s="32">
+      <c r="B27" s="40"/>
+      <c r="C27" s="40"/>
+      <c r="D27" s="33">
         <v>0</v>
       </c>
       <c r="E27" s="5" t="s">
@@ -2010,12 +1925,12 @@
       <c r="G27"/>
     </row>
     <row r="28" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A28" s="36" t="s">
+      <c r="A28" s="40" t="s">
         <v>21</v>
       </c>
-      <c r="B28" s="36"/>
-      <c r="C28" s="36"/>
-      <c r="D28" s="32">
+      <c r="B28" s="40"/>
+      <c r="C28" s="40"/>
+      <c r="D28" s="33">
         <v>0</v>
       </c>
       <c r="E28" s="5" t="s">
@@ -2025,12 +1940,12 @@
       <c r="G28"/>
     </row>
     <row r="29" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A29" s="36" t="s">
+      <c r="A29" s="40" t="s">
         <v>22</v>
       </c>
-      <c r="B29" s="36"/>
-      <c r="C29" s="36"/>
-      <c r="D29" s="32">
+      <c r="B29" s="40"/>
+      <c r="C29" s="40"/>
+      <c r="D29" s="33">
         <v>0</v>
       </c>
       <c r="E29" s="5" t="s">
@@ -2040,13 +1955,13 @@
       <c r="G29"/>
     </row>
     <row r="30" spans="1:7" ht="32" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A30" s="33" t="s">
+      <c r="A30" s="38" t="s">
         <v>23</v>
       </c>
-      <c r="B30" s="33"/>
-      <c r="C30" s="33"/>
-      <c r="D30" s="32">
-        <v>0</v>
+      <c r="B30" s="38"/>
+      <c r="C30" s="38"/>
+      <c r="D30" s="33" t="s">
+        <v>38</v>
       </c>
       <c r="E30" s="5" t="s">
         <v>13</v>
@@ -2082,7 +1997,7 @@
       <c r="G33"/>
     </row>
     <row r="34" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A34" s="28" t="s">
+      <c r="A34" s="19" t="s">
         <v>24</v>
       </c>
       <c r="B34" s="2"/>
@@ -2093,7 +2008,7 @@
       <c r="G34"/>
     </row>
     <row r="35" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A35" s="28" t="s">
+      <c r="A35" s="19" t="s">
         <v>25</v>
       </c>
       <c r="B35" s="6"/>
@@ -2113,13 +2028,13 @@
       <c r="G36"/>
     </row>
     <row r="37" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A37" s="29" t="s">
+      <c r="A37" s="20" t="s">
         <v>26</v>
       </c>
       <c r="B37" s="9"/>
       <c r="C37" s="9"/>
       <c r="D37" s="9"/>
-      <c r="E37" s="18" t="s">
+      <c r="E37" s="12" t="s">
         <v>27</v>
       </c>
       <c r="F37"/>
@@ -2131,8 +2046,8 @@
       </c>
       <c r="B38" s="2"/>
       <c r="C38" s="2"/>
-      <c r="D38" s="17"/>
-      <c r="E38" s="17"/>
+      <c r="D38" s="11"/>
+      <c r="E38" s="11"/>
       <c r="F38"/>
       <c r="G38"/>
     </row>
@@ -2140,8 +2055,8 @@
       <c r="A39" s="2"/>
       <c r="B39" s="2"/>
       <c r="C39" s="2"/>
-      <c r="D39" s="17"/>
-      <c r="E39" s="17"/>
+      <c r="D39" s="11"/>
+      <c r="E39" s="11"/>
       <c r="F39"/>
       <c r="G39"/>
     </row>
@@ -2166,7 +2081,7 @@
       <c r="C41" s="2"/>
       <c r="D41" s="2"/>
       <c r="E41" s="10" t="s">
-        <v>38</v>
+        <v>43</v>
       </c>
       <c r="F41"/>
       <c r="G41"/>
@@ -2201,7 +2116,7 @@
       <c r="C44" s="2"/>
       <c r="D44" s="2"/>
       <c r="E44" s="10" t="s">
-        <v>39</v>
+        <v>34</v>
       </c>
       <c r="F44"/>
       <c r="G44"/>
@@ -2238,19 +2153,11 @@
       <c r="G47"/>
     </row>
     <row r="48" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A48" s="22" t="s">
-        <v>49</v>
-      </c>
+      <c r="A48" s="14"/>
       <c r="B48" s="9"/>
-      <c r="C48" s="40" t="s">
-        <v>41</v>
-      </c>
-      <c r="D48" s="23" t="s">
-        <v>9</v>
-      </c>
-      <c r="E48" s="40" t="s">
-        <v>42</v>
-      </c>
+      <c r="C48" s="25"/>
+      <c r="D48" s="15"/>
+      <c r="E48" s="25"/>
       <c r="F48"/>
       <c r="G48"/>
     </row>
@@ -2273,28 +2180,20 @@
       <c r="G50"/>
     </row>
     <row r="51" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A51" s="3" t="s">
-        <v>2</v>
-      </c>
+      <c r="A51" s="22"/>
       <c r="B51" s="2"/>
       <c r="C51" s="2"/>
       <c r="D51" s="2"/>
-      <c r="E51" s="18"/>
+      <c r="E51" s="12"/>
       <c r="F51"/>
       <c r="G51"/>
     </row>
     <row r="52" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A52" s="3" t="s">
-        <v>4</v>
-      </c>
+      <c r="A52" s="22"/>
       <c r="B52" s="2"/>
       <c r="C52" s="2"/>
-      <c r="D52" s="17" t="s">
-        <v>34</v>
-      </c>
-      <c r="E52" s="30" t="s">
-        <v>38</v>
-      </c>
+      <c r="D52" s="11"/>
+      <c r="E52" s="21"/>
       <c r="F52"/>
       <c r="G52"/>
     </row>
@@ -2302,113 +2201,80 @@
       <c r="A53" s="2"/>
       <c r="B53" s="9"/>
       <c r="C53" s="2"/>
-      <c r="D53" s="17"/>
-      <c r="E53" s="17"/>
+      <c r="D53" s="11"/>
+      <c r="E53" s="11"/>
       <c r="F53"/>
       <c r="G53"/>
     </row>
     <row r="54" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A54" s="2"/>
-      <c r="B54" s="21"/>
+      <c r="B54" s="13"/>
       <c r="C54" s="2"/>
-      <c r="D54" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="E54" s="24" t="s">
-        <v>38</v>
-      </c>
+      <c r="D54" s="22"/>
+      <c r="E54" s="16"/>
       <c r="F54"/>
       <c r="G54"/>
     </row>
     <row r="55" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A55" s="2"/>
       <c r="B55" s="2"/>
-      <c r="C55" s="26"/>
-      <c r="D55" s="26"/>
-      <c r="E55" s="26"/>
+      <c r="C55" s="17"/>
+      <c r="D55" s="17"/>
+      <c r="E55" s="17"/>
       <c r="F55"/>
       <c r="G55"/>
     </row>
     <row r="56" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A56" s="2"/>
       <c r="B56" s="2"/>
-      <c r="C56" s="26"/>
-      <c r="D56" s="26"/>
-      <c r="E56" s="26"/>
+      <c r="C56" s="17"/>
+      <c r="D56" s="17"/>
+      <c r="E56" s="17"/>
       <c r="F56"/>
       <c r="G56"/>
     </row>
     <row r="57" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A57" s="31" t="s">
-        <v>17</v>
-      </c>
-      <c r="B57" s="11"/>
-      <c r="C57" s="11"/>
-      <c r="D57" s="11"/>
-      <c r="E57" s="11"/>
+      <c r="A57" s="22"/>
+      <c r="B57" s="2"/>
+      <c r="C57" s="2"/>
+      <c r="D57" s="2"/>
+      <c r="E57" s="2"/>
       <c r="F57"/>
       <c r="G57"/>
     </row>
     <row r="58" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A58" s="12" t="s">
-        <v>46</v>
-      </c>
-      <c r="B58" s="12" t="s">
-        <v>50</v>
-      </c>
-      <c r="C58" s="13" t="s">
-        <v>35</v>
-      </c>
-      <c r="D58" s="13" t="s">
-        <v>45</v>
-      </c>
-      <c r="E58" s="13" t="s">
-        <v>36</v>
-      </c>
+      <c r="A58" s="20"/>
+      <c r="B58" s="20"/>
+      <c r="C58" s="26"/>
+      <c r="D58" s="26"/>
+      <c r="E58" s="26"/>
       <c r="F58"/>
       <c r="G58"/>
     </row>
     <row r="59" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A59" s="14" t="s">
-        <v>47</v>
-      </c>
-      <c r="B59" s="25" t="s">
-        <v>48</v>
-      </c>
-      <c r="C59" s="20" t="s">
-        <v>43</v>
-      </c>
-      <c r="D59" s="20" t="s">
-        <v>44</v>
-      </c>
-      <c r="E59" s="20" t="e">
-        <f>C59-D59</f>
-        <v>#VALUE!</v>
-      </c>
+      <c r="A59" s="27"/>
+      <c r="B59" s="28"/>
+      <c r="C59" s="29"/>
+      <c r="D59" s="29"/>
+      <c r="E59" s="29"/>
       <c r="F59"/>
       <c r="G59"/>
     </row>
     <row r="60" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A60" s="15" t="s">
-        <v>37</v>
-      </c>
-      <c r="B60" s="16"/>
-      <c r="C60" s="19">
-        <f>SUM(C59)</f>
-        <v>0</v>
-      </c>
-      <c r="D60" s="19">
-        <f>SUM(D59)</f>
-        <v>0</v>
-      </c>
-      <c r="E60" s="20" t="e">
-        <f>SUM(E59)</f>
-        <v>#VALUE!</v>
-      </c>
+      <c r="A60" s="22"/>
+      <c r="B60" s="2"/>
+      <c r="C60" s="30"/>
+      <c r="D60" s="30"/>
+      <c r="E60" s="29"/>
       <c r="F60"/>
       <c r="G60"/>
     </row>
     <row r="61" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A61" s="31"/>
+      <c r="B61" s="31"/>
+      <c r="C61" s="31"/>
+      <c r="D61" s="31"/>
+      <c r="E61" s="31"/>
       <c r="F61"/>
       <c r="G61"/>
     </row>
@@ -2539,7 +2405,6 @@
   </sheetData>
   <mergeCells count="10">
     <mergeCell ref="A30:C30"/>
-    <mergeCell ref="A2:E2"/>
     <mergeCell ref="A1:E1"/>
     <mergeCell ref="A24:C24"/>
     <mergeCell ref="A25:C25"/>
@@ -2548,8 +2413,9 @@
     <mergeCell ref="A28:C28"/>
     <mergeCell ref="A29:C29"/>
     <mergeCell ref="A4:E4"/>
+    <mergeCell ref="A2:C2"/>
   </mergeCells>
-  <phoneticPr fontId="5" type="noConversion"/>
+  <phoneticPr fontId="4" type="noConversion"/>
   <pageMargins left="0.70866099999999999" right="0.31496099999999999" top="0.748031" bottom="0.748031" header="0.31496099999999999" footer="0.31496099999999999"/>
   <pageSetup paperSize="9" orientation="portrait"/>
   <headerFooter>

</xml_diff>

<commit_message>
Add scheduler, party representation and other
</commit_message>
<xml_diff>
--- a/src/main/resources/templates/provision_of_service_act.xlsx
+++ b/src/main/resources/templates/provision_of_service_act.xlsx
@@ -155,15 +155,6 @@
     <t>м.п.</t>
   </si>
   <si>
-    <t xml:space="preserve">??? </t>
-  </si>
-  <si>
-    <t>${shopAccounting.fromTime}</t>
-  </si>
-  <si>
-    <t>${shopAccounting.toTime}</t>
-  </si>
-  <si>
     <t>${shopAccounting.openingBalance}</t>
   </si>
   <si>
@@ -176,19 +167,28 @@
     <t>${shopAccounting.feeCharged}</t>
   </si>
   <si>
-    <t>${shopAccounting.merchantId}</t>
-  </si>
-  <si>
-    <t>${shopAccounting.merchantName}</t>
-  </si>
-  <si>
-    <t>${shopAccounting.merchantRepresentativePosition} ${shopAccounting.merchantRepresentativeFullName}</t>
-  </si>
-  <si>
-    <t>${shopAccounting.merchantContractCreatedAt}</t>
-  </si>
-  <si>
-    <t>к Договору № ${shopAccounting.merchantContractId} от</t>
+    <t>${toTime}</t>
+  </si>
+  <si>
+    <t>${fromTime}</t>
+  </si>
+  <si>
+    <t>${partyRepresentation.merchantContractCreatedAt}</t>
+  </si>
+  <si>
+    <t>${partyRepresentation.merchantName}</t>
+  </si>
+  <si>
+    <t>${partyRepresentation.merchantId}</t>
+  </si>
+  <si>
+    <t>к Договору № ${partyRepresentation.merchantContractId} от</t>
+  </si>
+  <si>
+    <t>${partyRepresentation.merchantRepresentativePosition} ${partyRepresentation.merchantRepresentativeFullName}</t>
+  </si>
+  <si>
+    <t>${partyRepresentation.merchantRepresentativeDocument}</t>
   </si>
 </sst>
 </file>
@@ -1600,8 +1600,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G92"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" view="pageBreakPreview" zoomScale="60" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:C2"/>
+    <sheetView showGridLines="0" tabSelected="1" view="pageBreakPreview" topLeftCell="A9" zoomScale="60" workbookViewId="0">
+      <selection activeCell="C38" sqref="C38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1625,12 +1625,12 @@
     </row>
     <row r="2" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="42" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="B2" s="42"/>
       <c r="C2" s="42"/>
       <c r="D2" s="37" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="E2" s="36"/>
       <c r="F2"/>
@@ -1675,7 +1675,7 @@
       <c r="C6" s="2"/>
       <c r="D6" s="10"/>
       <c r="E6" s="35" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="F6"/>
       <c r="G6"/>
@@ -1694,7 +1694,7 @@
       <c r="C8" s="2"/>
       <c r="D8" s="10"/>
       <c r="E8" s="16" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="F8"/>
       <c r="G8"/>
@@ -1762,13 +1762,13 @@
         <v>8</v>
       </c>
       <c r="B15" s="24" t="s">
-        <v>35</v>
+        <v>39</v>
       </c>
       <c r="C15" s="18" t="s">
         <v>9</v>
       </c>
       <c r="D15" s="23" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="E15" s="3" t="s">
         <v>10</v>
@@ -1803,7 +1803,7 @@
       <c r="B18" s="2"/>
       <c r="C18" s="2"/>
       <c r="D18" s="33" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="E18" s="5" t="s">
         <v>13</v>
@@ -1827,7 +1827,7 @@
       <c r="B20" s="2"/>
       <c r="C20" s="2"/>
       <c r="D20" s="33" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="E20" s="5" t="s">
         <v>13</v>
@@ -1871,7 +1871,7 @@
       <c r="B24" s="38"/>
       <c r="C24" s="38"/>
       <c r="D24" s="33" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="E24" s="5" t="s">
         <v>13</v>
@@ -1886,7 +1886,7 @@
       <c r="B25" s="40"/>
       <c r="C25" s="40"/>
       <c r="D25" s="33" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="E25" s="5" t="s">
         <v>18</v>
@@ -1901,7 +1901,7 @@
       <c r="B26" s="40"/>
       <c r="C26" s="40"/>
       <c r="D26" s="33" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="E26" s="5" t="s">
         <v>18</v>
@@ -1961,7 +1961,7 @@
       <c r="B30" s="38"/>
       <c r="C30" s="38"/>
       <c r="D30" s="33" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="E30" s="5" t="s">
         <v>13</v>
@@ -2081,7 +2081,7 @@
       <c r="C41" s="2"/>
       <c r="D41" s="2"/>
       <c r="E41" s="10" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="F41"/>
       <c r="G41"/>
@@ -2116,7 +2116,7 @@
       <c r="C44" s="2"/>
       <c r="D44" s="2"/>
       <c r="E44" s="10" t="s">
-        <v>34</v>
+        <v>45</v>
       </c>
       <c r="F44"/>
       <c r="G44"/>

</xml_diff>

<commit_message>
MST-108: Add values to report template
</commit_message>
<xml_diff>
--- a/src/main/resources/templates/provision_of_service_act.xlsx
+++ b/src/main/resources/templates/provision_of_service_act.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="28502"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="28702"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -51,7 +51,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="48">
   <si>
     <t>Акт об оказании услуг</t>
   </si>
@@ -189,6 +189,12 @@
   </si>
   <si>
     <t>${partyRepresentation.merchantRepresentativeDocument}</t>
+  </si>
+  <si>
+    <t>${shopAccounting.fundsPaidOut}</t>
+  </si>
+  <si>
+    <t>${shopAccounting.fundsRefunded}</t>
   </si>
 </sst>
 </file>
@@ -1601,7 +1607,7 @@
   <dimension ref="A1:G92"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" view="pageBreakPreview" topLeftCell="A9" zoomScale="60" workbookViewId="0">
-      <selection activeCell="C38" sqref="C38"/>
+      <selection activeCell="D23" sqref="D23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1915,8 +1921,8 @@
       </c>
       <c r="B27" s="40"/>
       <c r="C27" s="40"/>
-      <c r="D27" s="33">
-        <v>0</v>
+      <c r="D27" s="33" t="s">
+        <v>46</v>
       </c>
       <c r="E27" s="5" t="s">
         <v>18</v>
@@ -1945,8 +1951,8 @@
       </c>
       <c r="B29" s="40"/>
       <c r="C29" s="40"/>
-      <c r="D29" s="33">
-        <v>0</v>
+      <c r="D29" s="33" t="s">
+        <v>47</v>
       </c>
       <c r="E29" s="5" t="s">
         <v>13</v>

</xml_diff>

<commit_message>
MST-108: added fundsPaidOut and fundsRefunded (#6)
* MST-108: added fundsPaidOut and fundsRefunded

* MST-108: Add values to report template

* MST-108: Some fixes

* MST_108: Add new rule in mockito
</commit_message>
<xml_diff>
--- a/src/main/resources/templates/provision_of_service_act.xlsx
+++ b/src/main/resources/templates/provision_of_service_act.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="28502"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="28702"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -51,7 +51,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="48">
   <si>
     <t>Акт об оказании услуг</t>
   </si>
@@ -189,6 +189,12 @@
   </si>
   <si>
     <t>${partyRepresentation.merchantRepresentativeDocument}</t>
+  </si>
+  <si>
+    <t>${shopAccounting.fundsPaidOut}</t>
+  </si>
+  <si>
+    <t>${shopAccounting.fundsRefunded}</t>
   </si>
 </sst>
 </file>
@@ -1600,8 +1606,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G92"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" view="pageBreakPreview" topLeftCell="A9" zoomScale="60" workbookViewId="0">
-      <selection activeCell="C38" sqref="C38"/>
+    <sheetView showGridLines="0" tabSelected="1" view="pageBreakPreview" zoomScale="60" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1915,8 +1921,8 @@
       </c>
       <c r="B27" s="40"/>
       <c r="C27" s="40"/>
-      <c r="D27" s="33">
-        <v>0</v>
+      <c r="D27" s="33" t="s">
+        <v>46</v>
       </c>
       <c r="E27" s="5" t="s">
         <v>18</v>
@@ -1945,8 +1951,8 @@
       </c>
       <c r="B29" s="40"/>
       <c r="C29" s="40"/>
-      <c r="D29" s="33">
-        <v>0</v>
+      <c r="D29" s="33" t="s">
+        <v>47</v>
       </c>
       <c r="E29" s="5" t="s">
         <v>13</v>

</xml_diff>

<commit_message>
Change date format to "dd.mm.yyyy"
</commit_message>
<xml_diff>
--- a/src/main/resources/templates/provision_of_service_act.xlsx
+++ b/src/main/resources/templates/provision_of_service_act.xlsx
@@ -201,9 +201,8 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <numFmts count="3">
+  <numFmts count="2">
     <numFmt numFmtId="164" formatCode="#,##0.00&quot; &quot;;&quot;-&quot;#,##0.00&quot; &quot;"/>
-    <numFmt numFmtId="165" formatCode="[$-FC19]dd\ mmmm\ yyyy\ \г\.;@"/>
     <numFmt numFmtId="166" formatCode="dd\.mm\.yyyy"/>
   </numFmts>
   <fonts count="6" x14ac:knownFonts="1">
@@ -340,12 +339,6 @@
     <xf numFmtId="49" fontId="2" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="165" fontId="5" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="5" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="4" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
@@ -374,6 +367,12 @@
     </xf>
     <xf numFmtId="49" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="5" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="166" fontId="5" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1565,7 +1564,7 @@
   <dimension ref="A1:DZ234"/>
   <sheetViews>
     <sheetView tabSelected="1" view="pageBreakPreview" zoomScale="60" workbookViewId="0">
-      <selection activeCell="E12" sqref="E12"/>
+      <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1575,24 +1574,24 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:130" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="26" t="s">
+      <c r="A1" s="24" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="26"/>
-      <c r="C1" s="26"/>
-      <c r="D1" s="26"/>
-      <c r="E1" s="26"/>
+      <c r="B1" s="24"/>
+      <c r="C1" s="24"/>
+      <c r="D1" s="24"/>
+      <c r="E1" s="24"/>
     </row>
     <row r="2" spans="1:130" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="29" t="s">
+      <c r="A2" s="27" t="s">
         <v>42</v>
       </c>
-      <c r="B2" s="29"/>
-      <c r="C2" s="29"/>
-      <c r="D2" s="24" t="s">
+      <c r="B2" s="27"/>
+      <c r="C2" s="27"/>
+      <c r="D2" s="22" t="s">
         <v>47</v>
       </c>
-      <c r="E2" s="23"/>
+      <c r="E2" s="21"/>
     </row>
     <row r="3" spans="1:130" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="2"/>
@@ -1602,13 +1601,13 @@
       <c r="E3" s="2"/>
     </row>
     <row r="4" spans="1:130" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="28" t="s">
+      <c r="A4" s="26" t="s">
         <v>1</v>
       </c>
-      <c r="B4" s="28"/>
-      <c r="C4" s="28"/>
-      <c r="D4" s="28"/>
-      <c r="E4" s="28"/>
+      <c r="B4" s="26"/>
+      <c r="C4" s="26"/>
+      <c r="D4" s="26"/>
+      <c r="E4" s="26"/>
     </row>
     <row r="5" spans="1:130" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="2"/>
@@ -1626,7 +1625,7 @@
       <c r="B6" s="2"/>
       <c r="C6" s="2"/>
       <c r="D6" s="10"/>
-      <c r="E6" s="22" t="s">
+      <c r="E6" s="20" t="s">
         <v>40</v>
       </c>
     </row>
@@ -1783,7 +1782,7 @@
       <c r="A10" s="2"/>
       <c r="B10" s="2"/>
       <c r="C10" s="13"/>
-      <c r="D10" s="21"/>
+      <c r="D10" s="19"/>
       <c r="E10" s="13"/>
     </row>
     <row r="11" spans="1:130" ht="15" customHeight="1" x14ac:dyDescent="0.2">
@@ -1822,13 +1821,13 @@
       <c r="A15" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="B15" s="18" t="s">
+      <c r="B15" s="28" t="s">
         <v>39</v>
       </c>
       <c r="C15" s="14" t="s">
         <v>9</v>
       </c>
-      <c r="D15" s="17" t="s">
+      <c r="D15" s="29" t="s">
         <v>38</v>
       </c>
       <c r="E15" s="3" t="s">
@@ -1857,7 +1856,7 @@
       </c>
       <c r="B18" s="2"/>
       <c r="C18" s="2"/>
-      <c r="D18" s="20" t="s">
+      <c r="D18" s="18" t="s">
         <v>36</v>
       </c>
       <c r="E18" s="5" t="s">
@@ -1868,7 +1867,7 @@
       <c r="A19" s="2"/>
       <c r="B19" s="2"/>
       <c r="C19" s="2"/>
-      <c r="D19" s="19"/>
+      <c r="D19" s="17"/>
       <c r="E19" s="6"/>
     </row>
     <row r="20" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.2">
@@ -1877,7 +1876,7 @@
       </c>
       <c r="B20" s="2"/>
       <c r="C20" s="2"/>
-      <c r="D20" s="20" t="s">
+      <c r="D20" s="18" t="s">
         <v>37</v>
       </c>
       <c r="E20" s="5" t="s">
@@ -1908,12 +1907,12 @@
       <c r="E23"/>
     </row>
     <row r="24" spans="1:5" ht="31" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A24" s="25" t="s">
+      <c r="A24" s="23" t="s">
         <v>16</v>
       </c>
-      <c r="B24" s="25"/>
-      <c r="C24" s="25"/>
-      <c r="D24" s="20" t="s">
+      <c r="B24" s="23"/>
+      <c r="C24" s="23"/>
+      <c r="D24" s="18" t="s">
         <v>34</v>
       </c>
       <c r="E24" s="5" t="s">
@@ -1921,12 +1920,12 @@
       </c>
     </row>
     <row r="25" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A25" s="27" t="s">
+      <c r="A25" s="25" t="s">
         <v>17</v>
       </c>
-      <c r="B25" s="27"/>
-      <c r="C25" s="27"/>
-      <c r="D25" s="20" t="s">
+      <c r="B25" s="25"/>
+      <c r="C25" s="25"/>
+      <c r="D25" s="18" t="s">
         <v>36</v>
       </c>
       <c r="E25" s="5" t="s">
@@ -1934,12 +1933,12 @@
       </c>
     </row>
     <row r="26" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A26" s="27" t="s">
+      <c r="A26" s="25" t="s">
         <v>19</v>
       </c>
-      <c r="B26" s="27"/>
-      <c r="C26" s="27"/>
-      <c r="D26" s="20" t="s">
+      <c r="B26" s="25"/>
+      <c r="C26" s="25"/>
+      <c r="D26" s="18" t="s">
         <v>37</v>
       </c>
       <c r="E26" s="5" t="s">
@@ -1947,12 +1946,12 @@
       </c>
     </row>
     <row r="27" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A27" s="27" t="s">
+      <c r="A27" s="25" t="s">
         <v>20</v>
       </c>
-      <c r="B27" s="27"/>
-      <c r="C27" s="27"/>
-      <c r="D27" s="20" t="s">
+      <c r="B27" s="25"/>
+      <c r="C27" s="25"/>
+      <c r="D27" s="18" t="s">
         <v>45</v>
       </c>
       <c r="E27" s="5" t="s">
@@ -1960,12 +1959,12 @@
       </c>
     </row>
     <row r="28" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A28" s="27" t="s">
+      <c r="A28" s="25" t="s">
         <v>21</v>
       </c>
-      <c r="B28" s="27"/>
-      <c r="C28" s="27"/>
-      <c r="D28" s="20">
+      <c r="B28" s="25"/>
+      <c r="C28" s="25"/>
+      <c r="D28" s="18">
         <v>0</v>
       </c>
       <c r="E28" s="5" t="s">
@@ -1973,12 +1972,12 @@
       </c>
     </row>
     <row r="29" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A29" s="27" t="s">
+      <c r="A29" s="25" t="s">
         <v>22</v>
       </c>
-      <c r="B29" s="27"/>
-      <c r="C29" s="27"/>
-      <c r="D29" s="20" t="s">
+      <c r="B29" s="25"/>
+      <c r="C29" s="25"/>
+      <c r="D29" s="18" t="s">
         <v>46</v>
       </c>
       <c r="E29" s="5" t="s">
@@ -1986,12 +1985,12 @@
       </c>
     </row>
     <row r="30" spans="1:5" ht="32" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A30" s="25" t="s">
+      <c r="A30" s="23" t="s">
         <v>23</v>
       </c>
-      <c r="B30" s="25"/>
-      <c r="C30" s="25"/>
-      <c r="D30" s="20" t="s">
+      <c r="B30" s="23"/>
+      <c r="C30" s="23"/>
+      <c r="D30" s="18" t="s">
         <v>35</v>
       </c>
       <c r="E30" s="5" t="s">

</xml_diff>

<commit_message>
REP-13: Move name in template
</commit_message>
<xml_diff>
--- a/src/main/resources/templates/provision_of_service_act.xlsx
+++ b/src/main/resources/templates/provision_of_service_act.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="28702"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="29005"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -51,7 +51,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="49">
   <si>
     <t>Акт об оказании услуг</t>
   </si>
@@ -143,9 +143,6 @@
     <t>________________________</t>
   </si>
   <si>
-    <t>Председатель Правления Бурлаков К.В.</t>
-  </si>
-  <si>
     <t>действует на основании</t>
   </si>
   <si>
@@ -182,9 +179,6 @@
     <t>к Договору № ${partyRepresentation.merchantContractId} от</t>
   </si>
   <si>
-    <t>${partyRepresentation.merchantRepresentativePosition} ${partyRepresentation.merchantRepresentativeFullName}</t>
-  </si>
-  <si>
     <t>${shopAccounting.fundsPaidOut}</t>
   </si>
   <si>
@@ -192,6 +186,18 @@
   </si>
   <si>
     <t>${partyRepresentation.merchantContractSignedAt}</t>
+  </si>
+  <si>
+    <t>${partyRepresentation.merchantRepresentativePosition}</t>
+  </si>
+  <si>
+    <t>${partyRepresentation.merchantRepresentativeFullName}</t>
+  </si>
+  <si>
+    <t>Председатель Правления</t>
+  </si>
+  <si>
+    <t>Бурлаков К.В.</t>
   </si>
 </sst>
 </file>
@@ -1561,7 +1567,7 @@
   <dimension ref="A1:DZ234"/>
   <sheetViews>
     <sheetView tabSelected="1" view="pageBreakPreview" zoomScale="60" workbookViewId="0">
-      <selection activeCell="E10" sqref="E10"/>
+      <selection activeCell="H30" sqref="H30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1581,12 +1587,12 @@
     </row>
     <row r="2" spans="1:130" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="29" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B2" s="29"/>
       <c r="C2" s="29"/>
       <c r="D2" s="22" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="E2" s="21"/>
     </row>
@@ -1623,7 +1629,7 @@
       <c r="C6" s="2"/>
       <c r="D6" s="10"/>
       <c r="E6" s="20" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="7" spans="1:130" s="12" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
@@ -1765,7 +1771,7 @@
       <c r="C8" s="2"/>
       <c r="D8" s="10"/>
       <c r="E8" s="10" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="9" spans="1:130" ht="15" customHeight="1" x14ac:dyDescent="0.2">
@@ -1819,13 +1825,13 @@
         <v>8</v>
       </c>
       <c r="B15" s="23" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C15" s="14" t="s">
         <v>9</v>
       </c>
       <c r="D15" s="24" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="E15" s="3" t="s">
         <v>10</v>
@@ -1854,7 +1860,7 @@
       <c r="B18" s="2"/>
       <c r="C18" s="2"/>
       <c r="D18" s="18" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="E18" s="5" t="s">
         <v>13</v>
@@ -1874,7 +1880,7 @@
       <c r="B20" s="2"/>
       <c r="C20" s="2"/>
       <c r="D20" s="18" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="E20" s="5" t="s">
         <v>13</v>
@@ -1910,7 +1916,7 @@
       <c r="B24" s="25"/>
       <c r="C24" s="25"/>
       <c r="D24" s="18" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="E24" s="5" t="s">
         <v>13</v>
@@ -1923,7 +1929,7 @@
       <c r="B25" s="27"/>
       <c r="C25" s="27"/>
       <c r="D25" s="18" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="E25" s="5" t="s">
         <v>18</v>
@@ -1936,7 +1942,7 @@
       <c r="B26" s="27"/>
       <c r="C26" s="27"/>
       <c r="D26" s="18" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="E26" s="5" t="s">
         <v>18</v>
@@ -1949,7 +1955,7 @@
       <c r="B27" s="27"/>
       <c r="C27" s="27"/>
       <c r="D27" s="18" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="E27" s="5" t="s">
         <v>18</v>
@@ -1975,7 +1981,7 @@
       <c r="B29" s="27"/>
       <c r="C29" s="27"/>
       <c r="D29" s="18" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="E29" s="5" t="s">
         <v>13</v>
@@ -1988,7 +1994,7 @@
       <c r="B30" s="25"/>
       <c r="C30" s="25"/>
       <c r="D30" s="18" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="E30" s="5" t="s">
         <v>13</v>
@@ -2080,42 +2086,46 @@
     </row>
     <row r="41" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A41" s="3" t="s">
-        <v>30</v>
+        <v>47</v>
       </c>
       <c r="B41" s="2"/>
       <c r="C41" s="2"/>
       <c r="D41" s="2"/>
       <c r="E41" s="10" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
     </row>
     <row r="42" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A42" s="2"/>
+      <c r="A42" s="2" t="s">
+        <v>48</v>
+      </c>
       <c r="B42" s="2"/>
       <c r="C42" s="2"/>
       <c r="D42" s="2"/>
-      <c r="E42" s="8"/>
+      <c r="E42" s="8" t="s">
+        <v>46</v>
+      </c>
     </row>
     <row r="43" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A43" s="3" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B43" s="2"/>
       <c r="C43" s="2"/>
       <c r="D43" s="2"/>
       <c r="E43" s="10" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="44" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A44" s="3" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B44" s="2"/>
       <c r="C44" s="2"/>
       <c r="D44" s="2"/>
       <c r="E44" s="10" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="45" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.2">
@@ -2127,13 +2137,13 @@
     </row>
     <row r="46" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A46" s="3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B46" s="2"/>
       <c r="C46" s="2"/>
       <c r="D46" s="2"/>
       <c r="E46" s="10" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="47" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
New acts by contract id
</commit_message>
<xml_diff>
--- a/src/main/resources/templates/provision_of_service_act.xlsx
+++ b/src/main/resources/templates/provision_of_service_act.xlsx
@@ -152,61 +152,60 @@
     <t>м.п.</t>
   </si>
   <si>
-    <t>${shopAccounting.openingBalance}</t>
-  </si>
-  <si>
-    <t>${shopAccounting.closingBalance}</t>
-  </si>
-  <si>
-    <t>${shopAccounting.fundsAcquired}</t>
-  </si>
-  <si>
-    <t>${shopAccounting.feeCharged}</t>
-  </si>
-  <si>
-    <t>${toTime}</t>
-  </si>
-  <si>
-    <t>${fromTime}</t>
-  </si>
-  <si>
-    <t>${partyRepresentation.merchantName}</t>
-  </si>
-  <si>
-    <t>${partyRepresentation.merchantId}</t>
-  </si>
-  <si>
-    <t>к Договору № ${partyRepresentation.merchantContractId} от</t>
-  </si>
-  <si>
-    <t>${shopAccounting.fundsPaidOut}</t>
-  </si>
-  <si>
-    <t>${shopAccounting.fundsRefunded}</t>
-  </si>
-  <si>
-    <t>${partyRepresentation.merchantContractSignedAt}</t>
-  </si>
-  <si>
-    <t>${partyRepresentation.merchantRepresentativePosition}</t>
-  </si>
-  <si>
-    <t>${partyRepresentation.merchantRepresentativeFullName}</t>
-  </si>
-  <si>
     <t>Председатель Правления</t>
   </si>
   <si>
     <t>Бурлаков К.В.</t>
+  </si>
+  <si>
+    <t>${registered_name}</t>
+  </si>
+  <si>
+    <t>${party_id}</t>
+  </si>
+  <si>
+    <t>${from_time}</t>
+  </si>
+  <si>
+    <t>${to_time}</t>
+  </si>
+  <si>
+    <t>${funds_acquired}</t>
+  </si>
+  <si>
+    <t>${fee_charged}</t>
+  </si>
+  <si>
+    <t>${opening_balance}</t>
+  </si>
+  <si>
+    <t>${funds_paid_out}</t>
+  </si>
+  <si>
+    <t>${funds_refunded}</t>
+  </si>
+  <si>
+    <t>${closing_balance}</t>
+  </si>
+  <si>
+    <t>${representative_full_name}</t>
+  </si>
+  <si>
+    <t>${representative_position}</t>
+  </si>
+  <si>
+    <t>к Договору № ${legal_agreement_id} от</t>
+  </si>
+  <si>
+    <t>${legal_agreement_signed_at}</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <numFmts count="2">
+  <numFmts count="1">
     <numFmt numFmtId="164" formatCode="#,##0.00&quot; &quot;;&quot;-&quot;#,##0.00&quot; &quot;"/>
-    <numFmt numFmtId="165" formatCode="dd\.mm\.yyyy"/>
   </numFmts>
   <fonts count="6" x14ac:knownFonts="1">
     <font>
@@ -355,15 +354,6 @@
     <xf numFmtId="49" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="165" fontId="5" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="165" fontId="5" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="49" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
@@ -376,6 +366,15 @@
     </xf>
     <xf numFmtId="49" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="5" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="5" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1567,7 +1566,7 @@
   <dimension ref="A1:DZ234"/>
   <sheetViews>
     <sheetView tabSelected="1" view="pageBreakPreview" zoomScale="60" workbookViewId="0">
-      <selection activeCell="H30" sqref="H30"/>
+      <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1577,22 +1576,22 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:130" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="26" t="s">
+      <c r="A1" s="23" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="26"/>
-      <c r="C1" s="26"/>
-      <c r="D1" s="26"/>
-      <c r="E1" s="26"/>
+      <c r="B1" s="23"/>
+      <c r="C1" s="23"/>
+      <c r="D1" s="23"/>
+      <c r="E1" s="23"/>
     </row>
     <row r="2" spans="1:130" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="29" t="s">
-        <v>41</v>
-      </c>
-      <c r="B2" s="29"/>
-      <c r="C2" s="29"/>
-      <c r="D2" s="22" t="s">
-        <v>44</v>
+      <c r="A2" s="26" t="s">
+        <v>47</v>
+      </c>
+      <c r="B2" s="26"/>
+      <c r="C2" s="26"/>
+      <c r="D2" s="27" t="s">
+        <v>48</v>
       </c>
       <c r="E2" s="21"/>
     </row>
@@ -1604,13 +1603,13 @@
       <c r="E3" s="2"/>
     </row>
     <row r="4" spans="1:130" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="28" t="s">
+      <c r="A4" s="25" t="s">
         <v>1</v>
       </c>
-      <c r="B4" s="28"/>
-      <c r="C4" s="28"/>
-      <c r="D4" s="28"/>
-      <c r="E4" s="28"/>
+      <c r="B4" s="25"/>
+      <c r="C4" s="25"/>
+      <c r="D4" s="25"/>
+      <c r="E4" s="25"/>
     </row>
     <row r="5" spans="1:130" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="2"/>
@@ -1629,7 +1628,7 @@
       <c r="C6" s="2"/>
       <c r="D6" s="10"/>
       <c r="E6" s="20" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
     </row>
     <row r="7" spans="1:130" s="12" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
@@ -1771,7 +1770,7 @@
       <c r="C8" s="2"/>
       <c r="D8" s="10"/>
       <c r="E8" s="10" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
     </row>
     <row r="9" spans="1:130" ht="15" customHeight="1" x14ac:dyDescent="0.2">
@@ -1824,14 +1823,14 @@
       <c r="A15" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="B15" s="23" t="s">
-        <v>38</v>
+      <c r="B15" s="29" t="s">
+        <v>37</v>
       </c>
       <c r="C15" s="14" t="s">
         <v>9</v>
       </c>
-      <c r="D15" s="24" t="s">
-        <v>37</v>
+      <c r="D15" s="28" t="s">
+        <v>38</v>
       </c>
       <c r="E15" s="3" t="s">
         <v>10</v>
@@ -1860,7 +1859,7 @@
       <c r="B18" s="2"/>
       <c r="C18" s="2"/>
       <c r="D18" s="18" t="s">
-        <v>35</v>
+        <v>39</v>
       </c>
       <c r="E18" s="5" t="s">
         <v>13</v>
@@ -1880,7 +1879,7 @@
       <c r="B20" s="2"/>
       <c r="C20" s="2"/>
       <c r="D20" s="18" t="s">
-        <v>36</v>
+        <v>40</v>
       </c>
       <c r="E20" s="5" t="s">
         <v>13</v>
@@ -1910,50 +1909,50 @@
       <c r="E23"/>
     </row>
     <row r="24" spans="1:5" ht="31" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A24" s="25" t="s">
+      <c r="A24" s="22" t="s">
         <v>16</v>
       </c>
-      <c r="B24" s="25"/>
-      <c r="C24" s="25"/>
+      <c r="B24" s="22"/>
+      <c r="C24" s="22"/>
       <c r="D24" s="18" t="s">
-        <v>33</v>
+        <v>41</v>
       </c>
       <c r="E24" s="5" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="25" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A25" s="27" t="s">
+      <c r="A25" s="24" t="s">
         <v>17</v>
       </c>
-      <c r="B25" s="27"/>
-      <c r="C25" s="27"/>
+      <c r="B25" s="24"/>
+      <c r="C25" s="24"/>
       <c r="D25" s="18" t="s">
-        <v>35</v>
+        <v>39</v>
       </c>
       <c r="E25" s="5" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="26" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A26" s="27" t="s">
+      <c r="A26" s="24" t="s">
         <v>19</v>
       </c>
-      <c r="B26" s="27"/>
-      <c r="C26" s="27"/>
+      <c r="B26" s="24"/>
+      <c r="C26" s="24"/>
       <c r="D26" s="18" t="s">
-        <v>36</v>
+        <v>40</v>
       </c>
       <c r="E26" s="5" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="27" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A27" s="27" t="s">
+      <c r="A27" s="24" t="s">
         <v>20</v>
       </c>
-      <c r="B27" s="27"/>
-      <c r="C27" s="27"/>
+      <c r="B27" s="24"/>
+      <c r="C27" s="24"/>
       <c r="D27" s="18" t="s">
         <v>42</v>
       </c>
@@ -1962,11 +1961,11 @@
       </c>
     </row>
     <row r="28" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A28" s="27" t="s">
+      <c r="A28" s="24" t="s">
         <v>21</v>
       </c>
-      <c r="B28" s="27"/>
-      <c r="C28" s="27"/>
+      <c r="B28" s="24"/>
+      <c r="C28" s="24"/>
       <c r="D28" s="18">
         <v>0</v>
       </c>
@@ -1975,11 +1974,11 @@
       </c>
     </row>
     <row r="29" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A29" s="27" t="s">
+      <c r="A29" s="24" t="s">
         <v>22</v>
       </c>
-      <c r="B29" s="27"/>
-      <c r="C29" s="27"/>
+      <c r="B29" s="24"/>
+      <c r="C29" s="24"/>
       <c r="D29" s="18" t="s">
         <v>43</v>
       </c>
@@ -1988,13 +1987,13 @@
       </c>
     </row>
     <row r="30" spans="1:5" ht="32" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A30" s="25" t="s">
+      <c r="A30" s="22" t="s">
         <v>23</v>
       </c>
-      <c r="B30" s="25"/>
-      <c r="C30" s="25"/>
+      <c r="B30" s="22"/>
+      <c r="C30" s="22"/>
       <c r="D30" s="18" t="s">
-        <v>34</v>
+        <v>44</v>
       </c>
       <c r="E30" s="5" t="s">
         <v>13</v>
@@ -2086,24 +2085,24 @@
     </row>
     <row r="41" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A41" s="3" t="s">
-        <v>47</v>
+        <v>33</v>
       </c>
       <c r="B41" s="2"/>
       <c r="C41" s="2"/>
       <c r="D41" s="2"/>
       <c r="E41" s="10" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
     </row>
     <row r="42" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A42" s="2" t="s">
-        <v>48</v>
+        <v>34</v>
       </c>
       <c r="B42" s="2"/>
       <c r="C42" s="2"/>
       <c r="D42" s="2"/>
       <c r="E42" s="8" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="43" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
Add shop in report template, other fixes
</commit_message>
<xml_diff>
--- a/src/main/resources/templates/provision_of_service_act.xlsx
+++ b/src/main/resources/templates/provision_of_service_act.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="14120"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000"/>
   </bookViews>
   <sheets>
     <sheet name="List1" sheetId="1" r:id="rId1"/>
@@ -51,7 +51,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="51">
   <si>
     <t>Акт об оказании услуг</t>
   </si>
@@ -198,6 +198,12 @@
   </si>
   <si>
     <t>${legal_agreement_signed_at}</t>
+  </si>
+  <si>
+    <t>Идентификатор магазина:</t>
+  </si>
+  <si>
+    <t>${shop_id}</t>
   </si>
 </sst>
 </file>
@@ -297,7 +303,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="30">
+  <cellXfs count="31">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -355,6 +361,15 @@
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="5" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="5" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -367,14 +382,8 @@
     <xf numFmtId="49" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="5" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="5" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1566,7 +1575,7 @@
   <dimension ref="A1:DZ234"/>
   <sheetViews>
     <sheetView tabSelected="1" view="pageBreakPreview" zoomScale="60" workbookViewId="0">
-      <selection activeCell="B15" sqref="B15"/>
+      <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1576,21 +1585,21 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:130" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="23" t="s">
+      <c r="A1" s="26" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="23"/>
-      <c r="C1" s="23"/>
-      <c r="D1" s="23"/>
-      <c r="E1" s="23"/>
+      <c r="B1" s="26"/>
+      <c r="C1" s="26"/>
+      <c r="D1" s="26"/>
+      <c r="E1" s="26"/>
     </row>
     <row r="2" spans="1:130" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="26" t="s">
+      <c r="A2" s="29" t="s">
         <v>47</v>
       </c>
-      <c r="B2" s="26"/>
-      <c r="C2" s="26"/>
-      <c r="D2" s="27" t="s">
+      <c r="B2" s="29"/>
+      <c r="C2" s="29"/>
+      <c r="D2" s="22" t="s">
         <v>48</v>
       </c>
       <c r="E2" s="21"/>
@@ -1603,13 +1612,13 @@
       <c r="E3" s="2"/>
     </row>
     <row r="4" spans="1:130" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="25" t="s">
+      <c r="A4" s="28" t="s">
         <v>1</v>
       </c>
-      <c r="B4" s="25"/>
-      <c r="C4" s="25"/>
-      <c r="D4" s="25"/>
-      <c r="E4" s="25"/>
+      <c r="B4" s="28"/>
+      <c r="C4" s="28"/>
+      <c r="D4" s="28"/>
+      <c r="E4" s="28"/>
     </row>
     <row r="5" spans="1:130" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="2"/>
@@ -1777,15 +1786,19 @@
       <c r="A9" s="2"/>
       <c r="B9" s="2"/>
       <c r="C9" s="13"/>
-      <c r="D9" s="13"/>
-      <c r="E9" s="13"/>
+      <c r="D9" s="30" t="s">
+        <v>49</v>
+      </c>
+      <c r="E9" s="30"/>
     </row>
     <row r="10" spans="1:130" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="2"/>
       <c r="B10" s="2"/>
       <c r="C10" s="13"/>
       <c r="D10" s="19"/>
-      <c r="E10" s="13"/>
+      <c r="E10" s="13" t="s">
+        <v>50</v>
+      </c>
     </row>
     <row r="11" spans="1:130" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="2"/>
@@ -1823,13 +1836,13 @@
       <c r="A15" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="B15" s="29" t="s">
+      <c r="B15" s="24" t="s">
         <v>37</v>
       </c>
       <c r="C15" s="14" t="s">
         <v>9</v>
       </c>
-      <c r="D15" s="28" t="s">
+      <c r="D15" s="23" t="s">
         <v>38</v>
       </c>
       <c r="E15" s="3" t="s">
@@ -1909,11 +1922,11 @@
       <c r="E23"/>
     </row>
     <row r="24" spans="1:5" ht="31" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A24" s="22" t="s">
+      <c r="A24" s="25" t="s">
         <v>16</v>
       </c>
-      <c r="B24" s="22"/>
-      <c r="C24" s="22"/>
+      <c r="B24" s="25"/>
+      <c r="C24" s="25"/>
       <c r="D24" s="18" t="s">
         <v>41</v>
       </c>
@@ -1922,11 +1935,11 @@
       </c>
     </row>
     <row r="25" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A25" s="24" t="s">
+      <c r="A25" s="27" t="s">
         <v>17</v>
       </c>
-      <c r="B25" s="24"/>
-      <c r="C25" s="24"/>
+      <c r="B25" s="27"/>
+      <c r="C25" s="27"/>
       <c r="D25" s="18" t="s">
         <v>39</v>
       </c>
@@ -1935,11 +1948,11 @@
       </c>
     </row>
     <row r="26" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A26" s="24" t="s">
+      <c r="A26" s="27" t="s">
         <v>19</v>
       </c>
-      <c r="B26" s="24"/>
-      <c r="C26" s="24"/>
+      <c r="B26" s="27"/>
+      <c r="C26" s="27"/>
       <c r="D26" s="18" t="s">
         <v>40</v>
       </c>
@@ -1948,11 +1961,11 @@
       </c>
     </row>
     <row r="27" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A27" s="24" t="s">
+      <c r="A27" s="27" t="s">
         <v>20</v>
       </c>
-      <c r="B27" s="24"/>
-      <c r="C27" s="24"/>
+      <c r="B27" s="27"/>
+      <c r="C27" s="27"/>
       <c r="D27" s="18" t="s">
         <v>42</v>
       </c>
@@ -1961,11 +1974,11 @@
       </c>
     </row>
     <row r="28" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A28" s="24" t="s">
+      <c r="A28" s="27" t="s">
         <v>21</v>
       </c>
-      <c r="B28" s="24"/>
-      <c r="C28" s="24"/>
+      <c r="B28" s="27"/>
+      <c r="C28" s="27"/>
       <c r="D28" s="18">
         <v>0</v>
       </c>
@@ -1974,11 +1987,11 @@
       </c>
     </row>
     <row r="29" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A29" s="24" t="s">
+      <c r="A29" s="27" t="s">
         <v>22</v>
       </c>
-      <c r="B29" s="24"/>
-      <c r="C29" s="24"/>
+      <c r="B29" s="27"/>
+      <c r="C29" s="27"/>
       <c r="D29" s="18" t="s">
         <v>43</v>
       </c>
@@ -1987,11 +2000,11 @@
       </c>
     </row>
     <row r="30" spans="1:5" ht="32" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A30" s="22" t="s">
+      <c r="A30" s="25" t="s">
         <v>23</v>
       </c>
-      <c r="B30" s="22"/>
-      <c r="C30" s="22"/>
+      <c r="B30" s="25"/>
+      <c r="C30" s="25"/>
       <c r="D30" s="18" t="s">
         <v>44</v>
       </c>
@@ -3462,7 +3475,7 @@
       <c r="E234"/>
     </row>
   </sheetData>
-  <mergeCells count="10">
+  <mergeCells count="11">
     <mergeCell ref="A30:C30"/>
     <mergeCell ref="A1:E1"/>
     <mergeCell ref="A24:C24"/>
@@ -3473,6 +3486,7 @@
     <mergeCell ref="A29:C29"/>
     <mergeCell ref="A4:E4"/>
     <mergeCell ref="A2:C2"/>
+    <mergeCell ref="D9:E9"/>
   </mergeCells>
   <phoneticPr fontId="4" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Change sub name and position
</commit_message>
<xml_diff>
--- a/src/main/resources/templates/provision_of_service_act.xlsx
+++ b/src/main/resources/templates/provision_of_service_act.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10410"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10810"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/inalarsanukaev/git/reporter/src/main/resources/templates/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tolkonepiu/Projects/reporter/src/main/resources/templates/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1924D5C9-7AC5-B34F-95CD-5A549C0B747F}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3CECAEF5-5C33-E746-8521-AE4E1D68E236}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16480" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -201,13 +201,13 @@
     <t>${shop_id}</t>
   </si>
   <si>
-    <t>Заместитель Председателя Правления</t>
-  </si>
-  <si>
-    <t>Лебедева Л.В.</t>
-  </si>
-  <si>
     <t>Доверенность № 13 от 21.02.2020</t>
+  </si>
+  <si>
+    <t>Губайдулин Т.Ф.</t>
+  </si>
+  <si>
+    <t>Председатель Правления</t>
   </si>
 </sst>
 </file>
@@ -391,7 +391,7 @@
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Обычный" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultPivotStyle="PivotStyleMedium7"/>
@@ -1582,7 +1582,7 @@
   <dimension ref="A1:DZ234"/>
   <sheetViews>
     <sheetView tabSelected="1" view="pageBreakPreview" zoomScale="160" zoomScaleSheetLayoutView="160" workbookViewId="0">
-      <selection activeCell="B38" sqref="B38"/>
+      <selection activeCell="D9" sqref="D9:E9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -2105,7 +2105,7 @@
     </row>
     <row r="41" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A41" s="3" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="B41" s="2"/>
       <c r="C41" s="2"/>
@@ -2138,7 +2138,7 @@
     </row>
     <row r="44" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A44" s="3" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="B44" s="2"/>
       <c r="C44" s="2"/>

</xml_diff>

<commit_message>
BJ-999: Change signer in acts
</commit_message>
<xml_diff>
--- a/src/main/resources/templates/provision_of_service_act.xlsx
+++ b/src/main/resources/templates/provision_of_service_act.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10810"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10913"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tolkonepiu/Projects/reporter/src/main/resources/templates/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F084B5F0-130A-F049-A20F-282F578A2E94}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7FBAF213-BFA6-F345-9368-EB903AB3195D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16480" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -52,7 +52,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="53">
   <si>
     <t>Акт об оказании услуг</t>
   </si>
@@ -195,19 +195,22 @@
     <t>${shop_id}</t>
   </si>
   <si>
-    <t>Председатель Правления</t>
-  </si>
-  <si>
-    <t>действующий на основании Устава</t>
-  </si>
-  <si>
-    <t>Губайдулин Т.Ф.,</t>
-  </si>
-  <si>
     <t>${representative_full_name},</t>
   </si>
   <si>
     <t>действующий на основании</t>
+  </si>
+  <si>
+    <t>Главный бухгалтер</t>
+  </si>
+  <si>
+    <t>Кахно А.В.,</t>
+  </si>
+  <si>
+    <t>действующая на основании</t>
+  </si>
+  <si>
+    <t>Доверенности N 40 от 08.09.2020</t>
   </si>
 </sst>
 </file>
@@ -1593,8 +1596,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:DZ234"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageBreakPreview" topLeftCell="A24" zoomScale="160" zoomScaleSheetLayoutView="160" workbookViewId="0">
-      <selection activeCell="D36" sqref="D36"/>
+    <sheetView tabSelected="1" view="pageBreakPreview" topLeftCell="A30" zoomScale="160" zoomScaleSheetLayoutView="160" workbookViewId="0">
+      <selection activeCell="C40" sqref="C40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -2117,7 +2120,7 @@
     </row>
     <row r="41" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A41" s="3" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="B41" s="2"/>
       <c r="C41" s="2"/>
@@ -2128,28 +2131,30 @@
     </row>
     <row r="42" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A42" s="26" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="B42" s="2"/>
       <c r="C42" s="2"/>
       <c r="D42" s="2"/>
       <c r="E42" s="8" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
     </row>
     <row r="43" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A43" s="25" t="s">
-        <v>48</v>
+        <v>51</v>
       </c>
       <c r="B43" s="2"/>
       <c r="C43" s="2"/>
       <c r="D43" s="2"/>
       <c r="E43" s="10" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
     </row>
     <row r="44" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A44" s="3"/>
+      <c r="A44" s="3" t="s">
+        <v>52</v>
+      </c>
       <c r="B44" s="2"/>
       <c r="C44" s="2"/>
       <c r="D44" s="2"/>

</xml_diff>

<commit_message>
Change signer data again
</commit_message>
<xml_diff>
--- a/src/main/resources/templates/provision_of_service_act.xlsx
+++ b/src/main/resources/templates/provision_of_service_act.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="11213"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10111"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tolkonepiu/Projects/reporter/src/main/resources/templates/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6E95FCEC-5918-E54F-85F2-69CAE68A9083}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{06495F74-7FBA-6149-A7A8-B6F6D4B0E349}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16480" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -210,7 +210,7 @@
     <t>действующая на основании</t>
   </si>
   <si>
-    <t>Доверенности № 49 от 15.09.2020</t>
+    <t>Доверенности № 40 от 15.09.2020</t>
   </si>
 </sst>
 </file>
@@ -1596,8 +1596,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:DZ234"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageBreakPreview" topLeftCell="A25" zoomScale="160" zoomScaleSheetLayoutView="160" workbookViewId="0">
-      <selection activeCell="B34" sqref="B34"/>
+    <sheetView tabSelected="1" view="pageBreakPreview" topLeftCell="A28" zoomScale="160" zoomScaleSheetLayoutView="160" workbookViewId="0">
+      <selection activeCell="B39" sqref="B39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>

</xml_diff>